<commit_message>
Uploaded updated parameter files
Updated files that run with the updated function to generate 2024 harvest estimates.
</commit_message>
<xml_diff>
--- a/CRC Data/CRC Estimate Function Inputs/CRC_Reporting_Rates.xlsx
+++ b/CRC Data/CRC Estimate Function Inputs/CRC_Reporting_Rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa.sharepoint.com/sites/DFW-TeamFPCrustyAll/Shared Documents/Recreational Fisheries/Catch Memos/CRC Data Analysis/CRC Data/CRC Estimate Function Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{AC9D3338-A214-49F3-A0F5-015DC57AFF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F23AC27-10CF-4D0F-AEE4-E5AF6EF7B600}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{AC9D3338-A214-49F3-A0F5-015DC57AFF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD6E7DFC-30D1-446E-82F6-9FBB12F481C1}"/>
   <bookViews>
-    <workbookView xWindow="8064" yWindow="612" windowWidth="14688" windowHeight="9576" xr2:uid="{419BAF26-5BC6-4352-9EBC-5A6389D0E4C9}"/>
+    <workbookView xWindow="5400" yWindow="48" windowWidth="17280" windowHeight="8880" xr2:uid="{419BAF26-5BC6-4352-9EBC-5A6389D0E4C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -146,7 +146,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -252,7 +252,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -394,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -405,7 +405,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,6 +732,12 @@
       <c r="C19">
         <v>81091</v>
       </c>
+      <c r="D19">
+        <v>33743</v>
+      </c>
+      <c r="E19">
+        <v>16660</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -739,6 +745,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="671c5c8a-d1dd-40a7-bcfd-3ed591bedb5d" xsi:nil="true"/>
@@ -751,7 +766,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE9114A9D0DECB469CD3434F7556ACE4" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ecdf13fd03e578e190d1c2fef808890a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="62120a19-a38a-4c78-8e86-03b65bdcf4fa" xmlns:ns3="671c5c8a-d1dd-40a7-bcfd-3ed591bedb5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d204db95074059abcc46212eb5d192a9" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1009,16 +1024,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39DF0C60-8600-4ABA-BCDA-512E931CADE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1BC7CAC-2F04-4EBF-9276-556CFC88EAC6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1030,7 +1044,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{054E103B-5DB1-4C20-8F5C-86EDDFB12D70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1048,12 +1062,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39DF0C60-8600-4ABA-BCDA-512E931CADE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>